<commit_message>
Actualización datos y limpieza programa 241123
</commit_message>
<xml_diff>
--- a/Datos_entrada/Base_Intro.xlsx
+++ b/Datos_entrada/Base_Intro.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bancolombia-my.sharepoint.com/personal/arygonza_bancolombia_com_co/Documents/Bancolombia_ARGO/Bancolombia_Argo2024/Personales/USabana/repos/Introduccion_R/Datos_entrada/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bancolombia-my.sharepoint.com/personal/arygonza_bancolombia_com_co/Documents/Bancolombia_ARGO/Bancolombia_Argo2024/Personales/USabana/repos/Seleccion_variables/Datos_entrada/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{8E6F181A-C039-4B6E-90DF-EC68636A57F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B8DA05A-266D-4066-BC51-E116DD940735}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{8E6F181A-C039-4B6E-90DF-EC68636A57F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F735BBE-6E32-4076-BF42-2062FCD9C2E7}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{89ED45F3-F60C-4443-A78A-EB8B08A8CC4B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{89ED45F3-F60C-4443-A78A-EB8B08A8CC4B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Base_LR" sheetId="1" r:id="rId1"/>
+    <sheet name="Base" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Base_LR!#REF!</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Base!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -196,12 +196,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -219,7 +225,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -239,6 +245,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8"/>
@@ -562,20 +571,20 @@
   <dimension ref="A1:R229"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="G209" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B211" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="R229" sqref="R229"/>
+      <selection pane="bottomRight" activeCell="B229" sqref="B229"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="17.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -631,7 +640,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -687,7 +696,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -743,12 +752,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>38718</v>
       </c>
       <c r="B4" s="3">
-        <v>68.303270745582964</v>
+        <v>68.30527596979978</v>
       </c>
       <c r="C4" s="3">
         <v>59.02</v>
@@ -799,12 +808,12 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>38749</v>
       </c>
       <c r="B5" s="3">
-        <v>66.849403033881316</v>
+        <v>66.857318142265271</v>
       </c>
       <c r="C5" s="3">
         <v>59.41</v>
@@ -855,12 +864,12 @@
         <v>4.37</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>38777</v>
       </c>
       <c r="B6" s="3">
-        <v>64.559640321042096</v>
+        <v>64.567234387692267</v>
       </c>
       <c r="C6" s="3">
         <v>59.83</v>
@@ -911,12 +920,12 @@
         <v>4.3099999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>38808</v>
       </c>
       <c r="B7" s="3">
-        <v>65.214128044408469</v>
+        <v>65.217871453638111</v>
       </c>
       <c r="C7" s="3">
         <v>60.09</v>
@@ -967,12 +976,12 @@
         <v>4.29</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>38838</v>
       </c>
       <c r="B8" s="3">
-        <v>66.012097956939328</v>
+        <v>66.012069004863235</v>
       </c>
       <c r="C8" s="3">
         <v>60.29</v>
@@ -1023,12 +1032,12 @@
         <v>4.29</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>38869</v>
       </c>
       <c r="B9" s="3">
-        <v>65.938281865186937</v>
+        <v>65.938212077219134</v>
       </c>
       <c r="C9" s="3">
         <v>60.48</v>
@@ -1079,12 +1088,12 @@
         <v>4.1900000000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>38899</v>
       </c>
       <c r="B10" s="3">
-        <v>67.347597176787886</v>
+        <v>67.350203866858237</v>
       </c>
       <c r="C10" s="3">
         <v>60.73</v>
@@ -1135,12 +1144,12 @@
         <v>4.17</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>38930</v>
       </c>
       <c r="B11" s="3">
-        <v>68.33758736282654</v>
+        <v>68.341029008813834</v>
       </c>
       <c r="C11" s="3">
         <v>60.96</v>
@@ -1191,12 +1200,12 @@
         <v>4.2799999999999994</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>38961</v>
       </c>
       <c r="B12" s="3">
-        <v>69.905208861606113</v>
+        <v>69.907562855130877</v>
       </c>
       <c r="C12" s="3">
         <v>61.14</v>
@@ -1247,12 +1256,12 @@
         <v>4.42</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>38991</v>
       </c>
       <c r="B13" s="3">
-        <v>70.790061640888382</v>
+        <v>70.781834982000305</v>
       </c>
       <c r="C13" s="3">
         <v>61.05</v>
@@ -1303,12 +1312,12 @@
         <v>4.49</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>39022</v>
       </c>
       <c r="B14" s="3">
-        <v>72.410616492632656</v>
+        <v>72.399273338577601</v>
       </c>
       <c r="C14" s="3">
         <v>61.19</v>
@@ -1359,12 +1368,12 @@
         <v>4.32</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>39052</v>
       </c>
       <c r="B15" s="3">
-        <v>74.455433061327412</v>
+        <v>74.445554789120322</v>
       </c>
       <c r="C15" s="3">
         <v>61.33</v>
@@ -1415,12 +1424,12 @@
         <v>4.2299999999999995</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>39083</v>
       </c>
       <c r="B16" s="3">
-        <v>72.773306054576679</v>
+        <v>72.775329213598539</v>
       </c>
       <c r="C16" s="3">
         <v>61.8</v>
@@ -1471,12 +1480,12 @@
         <v>4.1399999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>39114</v>
       </c>
       <c r="B17" s="3">
-        <v>70.765824022391868</v>
+        <v>70.774190797106428</v>
       </c>
       <c r="C17" s="3">
         <v>62.53</v>
@@ -1527,12 +1536,12 @@
         <v>4.17</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>39142</v>
       </c>
       <c r="B18" s="3">
-        <v>68.649632508079108</v>
+        <v>68.657819452488056</v>
       </c>
       <c r="C18" s="3">
         <v>63.29</v>
@@ -1583,12 +1592,12 @@
         <v>4.22</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>39173</v>
       </c>
       <c r="B19" s="3">
-        <v>69.3279362761062</v>
+        <v>69.332113676639537</v>
       </c>
       <c r="C19" s="3">
         <v>63.85</v>
@@ -1639,12 +1648,12 @@
         <v>4.43</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>39203</v>
       </c>
       <c r="B20" s="3">
-        <v>70.160683929306927</v>
+        <v>70.160866657550869</v>
       </c>
       <c r="C20" s="3">
         <v>64.05</v>
@@ -1695,12 +1704,12 @@
         <v>4.58</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>39234</v>
       </c>
       <c r="B21" s="3">
-        <v>70.334054408493373</v>
+        <v>70.334261105917719</v>
       </c>
       <c r="C21" s="3">
         <v>64.12</v>
@@ -1751,12 +1760,12 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>39264</v>
       </c>
       <c r="B22" s="3">
-        <v>71.904256769649933</v>
+        <v>71.907204982355537</v>
       </c>
       <c r="C22" s="3">
         <v>64.23</v>
@@ -1807,12 +1816,12 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>39295</v>
       </c>
       <c r="B23" s="3">
-        <v>72.874028853299151</v>
+        <v>72.877807896698428</v>
       </c>
       <c r="C23" s="3">
         <v>64.14</v>
@@ -1863,12 +1872,12 @@
         <v>4.3999999999999995</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>39326</v>
       </c>
       <c r="B24" s="3">
-        <v>74.134387427040693</v>
+        <v>74.136980130105925</v>
       </c>
       <c r="C24" s="3">
         <v>64.2</v>
@@ -1919,12 +1928,12 @@
         <v>4.3499999999999996</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>39356</v>
       </c>
       <c r="B25" s="3">
-        <v>75.064861282586989</v>
+        <v>75.055491746482232</v>
       </c>
       <c r="C25" s="3">
         <v>64.2</v>
@@ -1975,12 +1984,12 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>39387</v>
       </c>
       <c r="B26" s="3">
-        <v>76.760601545480412</v>
+        <v>76.747988167303859</v>
       </c>
       <c r="C26" s="3">
         <v>64.510000000000005</v>
@@ -2031,12 +2040,12 @@
         <v>4.3499999999999996</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>39417</v>
       </c>
       <c r="B27" s="3">
-        <v>79.078825770411513</v>
+        <v>79.067839425513</v>
       </c>
       <c r="C27" s="3">
         <v>64.819999999999993</v>
@@ -2087,12 +2096,12 @@
         <v>4.51</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>39448</v>
       </c>
       <c r="B28" s="3">
-        <v>77.333773631759456</v>
+        <v>77.336164865035983</v>
       </c>
       <c r="C28" s="3">
         <v>65.510000000000005</v>
@@ -2143,12 +2152,12 @@
         <v>4.6500000000000004</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>39479</v>
       </c>
       <c r="B29" s="3">
-        <v>75.307090607023568</v>
+        <v>75.316211275616851</v>
       </c>
       <c r="C29" s="3">
         <v>66.5</v>
@@ -2199,12 +2208,12 @@
         <v>4.78</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>39508</v>
       </c>
       <c r="B30" s="3">
-        <v>71.919860453753245</v>
+        <v>71.928490344871364</v>
       </c>
       <c r="C30" s="3">
         <v>67.040000000000006</v>
@@ -2255,12 +2264,12 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>39539</v>
       </c>
       <c r="B31" s="3">
-        <v>72.843015362616612</v>
+        <v>72.847179211162995</v>
       </c>
       <c r="C31" s="3">
         <v>67.510000000000005</v>
@@ -2311,12 +2320,12 @@
         <v>4.78</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>39569</v>
       </c>
       <c r="B32" s="3">
-        <v>73.019491935399941</v>
+        <v>73.019259482730419</v>
       </c>
       <c r="C32" s="3">
         <v>68.14</v>
@@ -2367,12 +2376,12 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>39600</v>
       </c>
       <c r="B33" s="3">
-        <v>73.544101050528923</v>
+        <v>73.543960741136758</v>
       </c>
       <c r="C33" s="3">
         <v>68.73</v>
@@ -2423,12 +2432,12 @@
         <v>5.33</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>39630</v>
       </c>
       <c r="B34" s="3">
-        <v>74.540214579407476</v>
+        <v>74.543150195349895</v>
       </c>
       <c r="C34" s="3">
         <v>69.06</v>
@@ -2479,12 +2488,12 @@
         <v>5.52</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>39661</v>
       </c>
       <c r="B35" s="3">
-        <v>75.39065673882817</v>
+        <v>75.394644063209583</v>
       </c>
       <c r="C35" s="3">
         <v>69.19</v>
@@ -2535,12 +2544,12 @@
         <v>5.71</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>39692</v>
       </c>
       <c r="B36" s="3">
-        <v>76.583083027298116</v>
+        <v>76.585921627161994</v>
       </c>
       <c r="C36" s="3">
         <v>69.06</v>
@@ -2591,12 +2600,12 @@
         <v>5.84</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>39722</v>
       </c>
       <c r="B37" s="3">
-        <v>76.853536185293294</v>
+        <v>76.844407672314262</v>
       </c>
       <c r="C37" s="3">
         <v>69.3</v>
@@ -2647,12 +2656,12 @@
         <v>5.36</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>39753</v>
       </c>
       <c r="B38" s="3">
-        <v>77.478147789796267</v>
+        <v>77.465283397360665</v>
       </c>
       <c r="C38" s="3">
         <v>69.489999999999995</v>
@@ -2703,12 +2712,12 @@
         <v>5.42</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>39783</v>
       </c>
       <c r="B39" s="3">
-        <v>79.188064147853979</v>
+        <v>79.176735966264175</v>
       </c>
       <c r="C39" s="3">
         <v>69.8</v>
@@ -2759,12 +2768,12 @@
         <v>5.36</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39814</v>
       </c>
       <c r="B40" s="3">
-        <v>76.630650378329207</v>
+        <v>76.632646179548033</v>
       </c>
       <c r="C40" s="3">
         <v>70.209999999999994</v>
@@ -2815,12 +2824,12 @@
         <v>5.2200000000000006</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>39845</v>
       </c>
       <c r="B41" s="3">
-        <v>74.712061785139369</v>
+        <v>74.721184655221037</v>
       </c>
       <c r="C41" s="3">
         <v>70.8</v>
@@ -2871,12 +2880,12 @@
         <v>4.97</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>39873</v>
       </c>
       <c r="B42" s="3">
-        <v>72.049021909781047</v>
+        <v>72.057677840857409</v>
       </c>
       <c r="C42" s="3">
         <v>71.150000000000006</v>
@@ -2927,12 +2936,12 @@
         <v>4.88</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>39904</v>
       </c>
       <c r="B43" s="3">
-        <v>73.191250222951126</v>
+        <v>73.195327410201486</v>
       </c>
       <c r="C43" s="3">
         <v>71.38</v>
@@ -2983,12 +2992,12 @@
         <v>4.66</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>39934</v>
       </c>
       <c r="B44" s="3">
-        <v>74.163903088858902</v>
+        <v>74.16368219752745</v>
       </c>
       <c r="C44" s="3">
         <v>71.39</v>
@@ -3039,12 +3048,12 @@
         <v>4.55</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>39965</v>
       </c>
       <c r="B45" s="3">
-        <v>74.243082632328409</v>
+        <v>74.243133365200052</v>
       </c>
       <c r="C45" s="3">
         <v>71.349999999999994</v>
@@ -3095,12 +3104,12 @@
         <v>4.51</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>39995</v>
       </c>
       <c r="B46" s="3">
-        <v>75.935014474415809</v>
+        <v>75.938471338155694</v>
       </c>
       <c r="C46" s="3">
         <v>71.319999999999993</v>
@@ -3151,12 +3160,12 @@
         <v>4.58</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>40026</v>
       </c>
       <c r="B47" s="3">
-        <v>76.316946795176776</v>
+        <v>76.321421097452586</v>
       </c>
       <c r="C47" s="3">
         <v>71.349999999999994</v>
@@ -3207,12 +3216,12 @@
         <v>4.5600000000000005</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>40057</v>
       </c>
       <c r="B48" s="3">
-        <v>77.384345128108862</v>
+        <v>77.38762818368248</v>
       </c>
       <c r="C48" s="3">
         <v>71.28</v>
@@ -3263,12 +3272,12 @@
         <v>4.42</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>40087</v>
       </c>
       <c r="B49" s="3">
-        <v>77.51080892777162</v>
+        <v>77.50105723629639</v>
       </c>
       <c r="C49" s="3">
         <v>71.19</v>
@@ -3319,12 +3328,12 @@
         <v>4.32</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>40118</v>
       </c>
       <c r="B50" s="3">
-        <v>79.096784149104181</v>
+        <v>79.083145095961115</v>
       </c>
       <c r="C50" s="3">
         <v>71.14</v>
@@ -3375,12 +3384,12 @@
         <v>3.9600000000000004</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>40148</v>
       </c>
       <c r="B51" s="3">
-        <v>81.823979462632096</v>
+        <v>81.811989743110431</v>
       </c>
       <c r="C51" s="3">
         <v>71.2</v>
@@ -3431,12 +3440,12 @@
         <v>3.63</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>40179</v>
       </c>
       <c r="B52" s="3">
-        <v>79.782050268034325</v>
+        <v>79.784414131623919</v>
       </c>
       <c r="C52" s="3">
         <v>71.69</v>
@@ -3487,12 +3496,12 @@
         <v>3.6799999999999997</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>40210</v>
       </c>
       <c r="B53" s="3">
-        <v>77.642342858282788</v>
+        <v>77.652096147821283</v>
       </c>
       <c r="C53" s="3">
         <v>72.28</v>
@@ -3543,12 +3552,12 @@
         <v>3.7900000000000005</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>40238</v>
       </c>
       <c r="B54" s="3">
-        <v>74.933183892048817</v>
+        <v>74.942221104681082</v>
       </c>
       <c r="C54" s="3">
         <v>72.459999999999994</v>
@@ -3599,12 +3608,12 @@
         <v>3.63</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>40269</v>
       </c>
       <c r="B55" s="3">
-        <v>76.219792427664842</v>
+        <v>76.223941808735219</v>
       </c>
       <c r="C55" s="3">
         <v>72.790000000000006</v>
@@ -3655,12 +3664,12 @@
         <v>3.58</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>40299</v>
       </c>
       <c r="B56" s="3">
-        <v>77.478339435800635</v>
+        <v>77.477911477168732</v>
       </c>
       <c r="C56" s="3">
         <v>72.87</v>
@@ -3711,12 +3720,12 @@
         <v>3.4000000000000004</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>40330</v>
       </c>
       <c r="B57" s="3">
-        <v>77.587784439258073</v>
+        <v>77.587714727810905</v>
       </c>
       <c r="C57" s="3">
         <v>72.95</v>
@@ -3767,12 +3776,12 @@
         <v>3.42</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>40360</v>
       </c>
       <c r="B58" s="3">
-        <v>78.794476327181158</v>
+        <v>78.797976129199029</v>
       </c>
       <c r="C58" s="3">
         <v>72.92</v>
@@ -3823,12 +3832,12 @@
         <v>3.34</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>40391</v>
       </c>
       <c r="B59" s="3">
-        <v>79.256249669201409</v>
+        <v>79.260832312304203</v>
       </c>
       <c r="C59" s="3">
         <v>73</v>
@@ -3879,12 +3888,12 @@
         <v>3.3300000000000005</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>40422</v>
       </c>
       <c r="B60" s="3">
-        <v>80.232356722860288</v>
+        <v>80.235677412443081</v>
       </c>
       <c r="C60" s="3">
         <v>72.900000000000006</v>
@@ -3935,12 +3944,12 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>40452</v>
       </c>
       <c r="B61" s="3">
-        <v>80.984938749387723</v>
+        <v>80.974766441329862</v>
       </c>
       <c r="C61" s="3">
         <v>72.84</v>
@@ -3991,12 +4000,12 @@
         <v>3.2</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>40483</v>
       </c>
       <c r="B62" s="3">
-        <v>82.769875644469849</v>
+        <v>82.755872105594264</v>
       </c>
       <c r="C62" s="3">
         <v>72.98</v>
@@ -4047,12 +4056,12 @@
         <v>3.15</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>40513</v>
       </c>
       <c r="B63" s="3">
-        <v>85.986571160018528</v>
+        <v>85.974282969250837</v>
       </c>
       <c r="C63" s="3">
         <v>73.45</v>
@@ -4103,12 +4112,12 @@
         <v>3.19</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>40544</v>
       </c>
       <c r="B64" s="3">
-        <v>84.501506636103315</v>
+        <v>84.504249676632909</v>
       </c>
       <c r="C64" s="3">
         <v>74.12</v>
@@ -4159,12 +4168,12 @@
         <v>3.4299999999999997</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>40575</v>
       </c>
       <c r="B65" s="3">
-        <v>82.425221330583454</v>
+        <v>82.435398150551165</v>
       </c>
       <c r="C65" s="3">
         <v>74.569999999999993</v>
@@ -4215,12 +4224,12 @@
         <v>3.42</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>40603</v>
       </c>
       <c r="B66" s="3">
-        <v>79.826509773334365</v>
+        <v>79.836098873406897</v>
       </c>
       <c r="C66" s="3">
         <v>74.77</v>
@@ -4271,12 +4280,12 @@
         <v>3.49</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>40634</v>
       </c>
       <c r="B67" s="3">
-        <v>80.845573888935462</v>
+        <v>80.850196044901949</v>
       </c>
       <c r="C67" s="3">
         <v>74.86</v>
@@ -4327,12 +4336,12 @@
         <v>3.4799999999999995</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>40664</v>
       </c>
       <c r="B68" s="3">
-        <v>82.406910332960749</v>
+        <v>82.406947169818352</v>
       </c>
       <c r="C68" s="3">
         <v>75.069999999999993</v>
@@ -4383,12 +4392,12 @@
         <v>3.36</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>40695</v>
       </c>
       <c r="B69" s="3">
-        <v>82.578005645838729</v>
+        <v>82.577988071800121</v>
       </c>
       <c r="C69" s="3">
         <v>75.31</v>
@@ -4439,12 +4448,12 @@
         <v>3.45</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>40725</v>
       </c>
       <c r="B70" s="3">
-        <v>84.137588189251403</v>
+        <v>84.140976876395442</v>
       </c>
       <c r="C70" s="3">
         <v>75.42</v>
@@ -4495,12 +4504,12 @@
         <v>3.46</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>40756</v>
       </c>
       <c r="B71" s="3">
-        <v>85.277537783753985</v>
+        <v>85.282216770229056</v>
       </c>
       <c r="C71" s="3">
         <v>75.39</v>
@@ -4551,12 +4560,12 @@
         <v>3.4000000000000004</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>40787</v>
       </c>
       <c r="B72" s="3">
-        <v>86.304449368126527</v>
+        <v>86.308149508435193</v>
       </c>
       <c r="C72" s="3">
         <v>75.62</v>
@@ -4607,12 +4616,12 @@
         <v>3.3300000000000005</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>40817</v>
       </c>
       <c r="B73" s="3">
-        <v>86.888393158470492</v>
+        <v>86.87841577083708</v>
       </c>
       <c r="C73" s="3">
         <v>75.77</v>
@@ -4663,12 +4672,12 @@
         <v>3.38</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>40848</v>
       </c>
       <c r="B74" s="3">
-        <v>88.198660296525986</v>
+        <v>88.184175672755643</v>
       </c>
       <c r="C74" s="3">
         <v>75.87</v>
@@ -4719,12 +4728,12 @@
         <v>3.4099999999999997</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>40878</v>
       </c>
       <c r="B75" s="3">
-        <v>91.121544847314567</v>
+        <v>91.108273180972006</v>
       </c>
       <c r="C75" s="3">
         <v>76.19</v>
@@ -4775,12 +4784,12 @@
         <v>3.44</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>40909</v>
       </c>
       <c r="B76" s="3">
-        <v>89.346955568300373</v>
+        <v>89.348773736550015</v>
       </c>
       <c r="C76" s="3">
         <v>76.75</v>
@@ -4831,12 +4840,12 @@
         <v>3.56</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>40940</v>
       </c>
       <c r="B77" s="3">
-        <v>87.145801917158749</v>
+        <v>87.15548995453257</v>
       </c>
       <c r="C77" s="3">
         <v>77.22</v>
@@ -4887,12 +4896,12 @@
         <v>3.61</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>40969</v>
       </c>
       <c r="B78" s="3">
-        <v>84.613099966172385</v>
+        <v>84.622567592064257</v>
       </c>
       <c r="C78" s="3">
         <v>77.31</v>
@@ -4943,12 +4952,12 @@
         <v>3.53</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>41000</v>
       </c>
       <c r="B79" s="3">
-        <v>85.461942058203022</v>
+        <v>85.466389745625563</v>
       </c>
       <c r="C79" s="3">
         <v>77.42</v>
@@ -4999,12 +5008,12 @@
         <v>3.45</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>41030</v>
       </c>
       <c r="B80" s="3">
-        <v>86.623861878423455</v>
+        <v>86.623508827609342</v>
       </c>
       <c r="C80" s="3">
         <v>77.66</v>
@@ -5055,12 +5064,12 @@
         <v>3.5000000000000004</v>
       </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>41061</v>
       </c>
       <c r="B81" s="3">
-        <v>86.59710975025861</v>
+        <v>86.59691129005023</v>
       </c>
       <c r="C81" s="3">
         <v>77.72</v>
@@ -5111,12 +5120,12 @@
         <v>3.54</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>41091</v>
       </c>
       <c r="B82" s="3">
-        <v>87.988583996124859</v>
+        <v>87.992021070577891</v>
       </c>
       <c r="C82" s="3">
         <v>77.7</v>
@@ -5167,12 +5176,12 @@
         <v>3.37</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>41122</v>
       </c>
       <c r="B83" s="3">
-        <v>87.821672097034067</v>
+        <v>87.826374658458903</v>
       </c>
       <c r="C83" s="3">
         <v>77.73</v>
@@ -5223,12 +5232,12 @@
         <v>3.27</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>41153</v>
       </c>
       <c r="B84" s="3">
-        <v>88.202334680656648</v>
+        <v>88.205937162785418</v>
       </c>
       <c r="C84" s="3">
         <v>77.959999999999994</v>
@@ -5279,12 +5288,12 @@
         <v>3.26</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>41183</v>
       </c>
       <c r="B85" s="3">
-        <v>88.379207743380519</v>
+        <v>88.368822772763451</v>
       </c>
       <c r="C85" s="3">
         <v>78.08</v>
@@ -5335,12 +5344,12 @@
         <v>3.2099999999999995</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>41214</v>
       </c>
       <c r="B86" s="3">
-        <v>90.469506948190642</v>
+        <v>90.455090961922437</v>
       </c>
       <c r="C86" s="3">
         <v>77.98</v>
@@ -5391,12 +5400,12 @@
         <v>3.2199999999999998</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>41244</v>
       </c>
       <c r="B87" s="3">
-        <v>93.517262609481406</v>
+        <v>93.504390961669131</v>
       </c>
       <c r="C87" s="3">
         <v>78.05</v>
@@ -5447,12 +5456,12 @@
         <v>3.1199999999999997</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>41275</v>
       </c>
       <c r="B88" s="3">
-        <v>92.255229515661128</v>
+        <v>92.25792885403969</v>
       </c>
       <c r="C88" s="3">
         <v>78.28</v>
@@ -5503,12 +5512,12 @@
         <v>2.8899999999999997</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>41306</v>
       </c>
       <c r="B89" s="3">
-        <v>89.815511304729839</v>
+        <v>89.826510391880447</v>
       </c>
       <c r="C89" s="3">
         <v>78.63</v>
@@ -5559,12 +5568,12 @@
         <v>2.85</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>41334</v>
       </c>
       <c r="B90" s="3">
-        <v>86.664609845292105</v>
+        <v>86.675278657079943</v>
       </c>
       <c r="C90" s="3">
         <v>78.790000000000006</v>
@@ -5615,12 +5624,12 @@
         <v>2.8899999999999997</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>41365</v>
       </c>
       <c r="B91" s="3">
-        <v>88.279240809654013</v>
+        <v>88.284359786101618</v>
       </c>
       <c r="C91" s="3">
         <v>78.989999999999995</v>
@@ -5671,12 +5680,12 @@
         <v>2.92</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>41395</v>
       </c>
       <c r="B92" s="3">
-        <v>90.314060988881224</v>
+        <v>90.313731999774106</v>
       </c>
       <c r="C92" s="3">
         <v>79.209999999999994</v>
@@ -5727,12 +5736,12 @@
         <v>3.01</v>
       </c>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>41426</v>
       </c>
       <c r="B93" s="3">
-        <v>91.395731026508585</v>
+        <v>91.395738762769312</v>
       </c>
       <c r="C93" s="3">
         <v>79.39</v>
@@ -5783,12 +5792,12 @@
         <v>3.09</v>
       </c>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>41456</v>
       </c>
       <c r="B94" s="3">
-        <v>92.915060016249797</v>
+        <v>92.919313665935746</v>
       </c>
       <c r="C94" s="3">
         <v>79.430000000000007</v>
@@ -5839,12 +5848,12 @@
         <v>3.05</v>
       </c>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>41487</v>
       </c>
       <c r="B95" s="3">
-        <v>93.201898153113333</v>
+        <v>93.207747021053137</v>
       </c>
       <c r="C95" s="3">
         <v>79.5</v>
@@ -5895,12 +5904,12 @@
         <v>3.0700000000000003</v>
       </c>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>41518</v>
       </c>
       <c r="B96" s="3">
-        <v>93.975098697427782</v>
+        <v>93.979613112671657</v>
       </c>
       <c r="C96" s="3">
         <v>79.73</v>
@@ -5951,12 +5960,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>41548</v>
       </c>
       <c r="B97" s="3">
-        <v>93.933826230049931</v>
+        <v>93.922213639261642</v>
       </c>
       <c r="C97" s="3">
         <v>79.52</v>
@@ -6007,12 +6016,12 @@
         <v>2.97</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>41579</v>
       </c>
       <c r="B98" s="3">
-        <v>95.971468992516677</v>
+        <v>95.954821962497704</v>
       </c>
       <c r="C98" s="3">
         <v>79.349999999999994</v>
@@ -6063,12 +6072,12 @@
         <v>2.92</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>41609</v>
       </c>
       <c r="B99" s="3">
-        <v>99.647541446262665</v>
+        <v>99.632350482970239</v>
       </c>
       <c r="C99" s="3">
         <v>79.56</v>
@@ -6119,12 +6128,12 @@
         <v>2.8899999999999997</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>41640</v>
       </c>
       <c r="B100" s="3">
-        <v>97.874285238981997</v>
+        <v>97.87680074282919</v>
       </c>
       <c r="C100" s="3">
         <v>79.95</v>
@@ -6175,12 +6184,12 @@
         <v>2.85</v>
       </c>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>41671</v>
       </c>
       <c r="B101" s="3">
-        <v>95.606619978969491</v>
+        <v>95.618276699826893</v>
       </c>
       <c r="C101" s="3">
         <v>80.45</v>
@@ -6231,12 +6240,12 @@
         <v>2.9000000000000004</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>41699</v>
       </c>
       <c r="B102" s="3">
-        <v>92.433413048019602</v>
+        <v>92.444674069941243</v>
       </c>
       <c r="C102" s="3">
         <v>80.77</v>
@@ -6287,12 +6296,12 @@
         <v>2.9899999999999998</v>
       </c>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>41730</v>
       </c>
       <c r="B103" s="3">
-        <v>93.499505093549701</v>
+        <v>93.504691092999678</v>
       </c>
       <c r="C103" s="3">
         <v>81.14</v>
@@ -6343,12 +6352,12 @@
         <v>3.1300000000000003</v>
       </c>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>41760</v>
       </c>
       <c r="B104" s="3">
-        <v>94.461732452343369</v>
+        <v>94.461258074517971</v>
       </c>
       <c r="C104" s="3">
         <v>81.53</v>
@@ -6399,12 +6408,12 @@
         <v>3.16</v>
       </c>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>41791</v>
       </c>
       <c r="B105" s="3">
-        <v>94.34612812589917</v>
+        <v>94.345916857676812</v>
       </c>
       <c r="C105" s="3">
         <v>81.61</v>
@@ -6455,12 +6464,12 @@
         <v>3.19</v>
       </c>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>41821</v>
       </c>
       <c r="B106" s="3">
-        <v>96.167724704947773</v>
+        <v>96.172171616396724</v>
       </c>
       <c r="C106" s="3">
         <v>81.73</v>
@@ -6511,12 +6520,12 @@
         <v>3.16</v>
       </c>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>41852</v>
       </c>
       <c r="B107" s="3">
-        <v>96.867431466510538</v>
+        <v>96.873374069542265</v>
       </c>
       <c r="C107" s="3">
         <v>81.900000000000006</v>
@@ -6567,12 +6576,12 @@
         <v>3.1399999999999997</v>
       </c>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>41883</v>
       </c>
       <c r="B108" s="3">
-        <v>97.95005302389329</v>
+        <v>97.954740471497999</v>
       </c>
       <c r="C108" s="3">
         <v>82.01</v>
@@ -6623,12 +6632,12 @@
         <v>3.16</v>
       </c>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>41913</v>
       </c>
       <c r="B109" s="3">
-        <v>98.231900370087487</v>
+        <v>98.219429687999423</v>
       </c>
       <c r="C109" s="3">
         <v>82.14</v>
@@ -6679,12 +6688,12 @@
         <v>3.15</v>
       </c>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>41944</v>
       </c>
       <c r="B110" s="3">
-        <v>99.808396407099679</v>
+        <v>99.790869173175381</v>
       </c>
       <c r="C110" s="3">
         <v>82.25</v>
@@ -6735,12 +6744,12 @@
         <v>3.1399999999999997</v>
       </c>
     </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>41974</v>
       </c>
       <c r="B111" s="3">
-        <v>103.32750853262274</v>
+        <v>103.3117713313185</v>
       </c>
       <c r="C111" s="3">
         <v>82.47</v>
@@ -6791,12 +6800,12 @@
         <v>3.2199999999999998</v>
       </c>
     </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>42005</v>
       </c>
       <c r="B112" s="3">
-        <v>101.04618420057449</v>
+        <v>101.04912211655947</v>
       </c>
       <c r="C112" s="3">
         <v>83</v>
@@ -6847,12 +6856,12 @@
         <v>3.3000000000000003</v>
       </c>
     </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>42036</v>
       </c>
       <c r="B113" s="3">
-        <v>98.563144649727917</v>
+        <v>98.575627498476692</v>
       </c>
       <c r="C113" s="3">
         <v>83.96</v>
@@ -6903,12 +6912,12 @@
         <v>3.18</v>
       </c>
     </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>42064</v>
       </c>
       <c r="B114" s="3">
-        <v>95.052847901744428</v>
+        <v>95.064831518258075</v>
       </c>
       <c r="C114" s="3">
         <v>84.45</v>
@@ -6959,12 +6968,12 @@
         <v>3.17</v>
       </c>
     </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>42095</v>
       </c>
       <c r="B115" s="3">
-        <v>96.292450760850727</v>
+        <v>96.298119509499656</v>
       </c>
       <c r="C115" s="3">
         <v>84.9</v>
@@ -7015,12 +7024,12 @@
         <v>3.1300000000000003</v>
       </c>
     </row>
-    <row r="116" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>42125</v>
       </c>
       <c r="B116" s="3">
-        <v>97.616098552083926</v>
+        <v>97.61576550905977</v>
       </c>
       <c r="C116" s="3">
         <v>85.12</v>
@@ -7071,12 +7080,12 @@
         <v>3.16</v>
       </c>
     </row>
-    <row r="117" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>42156</v>
       </c>
       <c r="B117" s="3">
-        <v>97.816902106902731</v>
+        <v>97.816679216499395</v>
       </c>
       <c r="C117" s="3">
         <v>85.21</v>
@@ -7127,12 +7136,12 @@
         <v>3.17</v>
       </c>
     </row>
-    <row r="118" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>42186</v>
       </c>
       <c r="B118" s="3">
-        <v>100.05318076181078</v>
+        <v>100.05819783917276</v>
       </c>
       <c r="C118" s="3">
         <v>85.37</v>
@@ -7183,12 +7192,12 @@
         <v>3.11</v>
       </c>
     </row>
-    <row r="119" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>42217</v>
       </c>
       <c r="B119" s="3">
-        <v>100.86706325367659</v>
+        <v>100.87399620271283</v>
       </c>
       <c r="C119" s="3">
         <v>85.78</v>
@@ -7239,12 +7248,12 @@
         <v>3.47</v>
       </c>
     </row>
-    <row r="120" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>42248</v>
       </c>
       <c r="B120" s="3">
-        <v>101.58299936507667</v>
+        <v>101.58856397863273</v>
       </c>
       <c r="C120" s="3">
         <v>86.39</v>
@@ -7295,12 +7304,12 @@
         <v>3.5999999999999996</v>
       </c>
     </row>
-    <row r="121" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>42278</v>
       </c>
       <c r="B121" s="3">
-        <v>101.13854143280416</v>
+        <v>101.12580527962204</v>
       </c>
       <c r="C121" s="3">
         <v>86.98</v>
@@ -7351,12 +7360,12 @@
         <v>4.12</v>
       </c>
     </row>
-    <row r="122" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>42309</v>
       </c>
       <c r="B122" s="3">
-        <v>102.27630818349536</v>
+        <v>102.2573991162717</v>
       </c>
       <c r="C122" s="3">
         <v>87.51</v>
@@ -7407,12 +7416,12 @@
         <v>4.41</v>
       </c>
     </row>
-    <row r="123" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>42339</v>
       </c>
       <c r="B123" s="3">
-        <v>105.54725062627612</v>
+        <v>105.52992528660978</v>
       </c>
       <c r="C123" s="3">
         <v>88.05</v>
@@ -7463,12 +7472,12 @@
         <v>4.63</v>
       </c>
     </row>
-    <row r="124" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>42370</v>
       </c>
       <c r="B124" s="3">
-        <v>103.05331173574798</v>
+        <v>103.05586968902635</v>
       </c>
       <c r="C124" s="3">
         <v>89.19</v>
@@ -7519,12 +7528,12 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="125" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>42401</v>
       </c>
       <c r="B125" s="3">
-        <v>101.18340877242339</v>
+        <v>101.19684175481598</v>
       </c>
       <c r="C125" s="3">
         <v>90.33</v>
@@ -7575,12 +7584,12 @@
         <v>4.54</v>
       </c>
     </row>
-    <row r="126" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>42430</v>
       </c>
       <c r="B126" s="3">
-        <v>97.398446939225082</v>
+        <v>97.411945831535377</v>
       </c>
       <c r="C126" s="3">
         <v>91.18</v>
@@ -7631,12 +7640,12 @@
         <v>4.41</v>
       </c>
     </row>
-    <row r="127" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>42461</v>
       </c>
       <c r="B127" s="3">
-        <v>99.020072910601755</v>
+        <v>99.026536505182364</v>
       </c>
       <c r="C127" s="3">
         <v>91.63</v>
@@ -7687,12 +7696,12 @@
         <v>4.54</v>
       </c>
     </row>
-    <row r="128" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
         <v>42491</v>
       </c>
       <c r="B128" s="3">
-        <v>99.535271251033393</v>
+        <v>99.535154853694067</v>
       </c>
       <c r="C128" s="3">
         <v>92.1</v>
@@ -7743,12 +7752,12 @@
         <v>4.53</v>
       </c>
     </row>
-    <row r="129" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <v>42522</v>
       </c>
       <c r="B129" s="3">
-        <v>100.10563169500405</v>
+        <v>100.10557872459061</v>
       </c>
       <c r="C129" s="3">
         <v>92.54</v>
@@ -7799,12 +7808,12 @@
         <v>4.37</v>
       </c>
     </row>
-    <row r="130" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
         <v>42552</v>
       </c>
       <c r="B130" s="3">
-        <v>100.88589412365967</v>
+        <v>100.89151631747443</v>
       </c>
       <c r="C130" s="3">
         <v>93.02</v>
@@ -7855,12 +7864,12 @@
         <v>4.6100000000000003</v>
       </c>
     </row>
-    <row r="131" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <v>42583</v>
       </c>
       <c r="B131" s="3">
-        <v>102.23587656536576</v>
+        <v>102.24356023285809</v>
       </c>
       <c r="C131" s="3">
         <v>92.73</v>
@@ -7911,12 +7920,12 @@
         <v>4.55</v>
       </c>
     </row>
-    <row r="132" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <v>42614</v>
       </c>
       <c r="B132" s="3">
-        <v>102.98030045406415</v>
+        <v>102.98654602904003</v>
       </c>
       <c r="C132" s="3">
         <v>92.68</v>
@@ -7967,12 +7976,12 @@
         <v>4.3499999999999996</v>
       </c>
     </row>
-    <row r="133" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
         <v>42644</v>
       </c>
       <c r="B133" s="3">
-        <v>103.51654748964371</v>
+        <v>103.50233684743709</v>
       </c>
       <c r="C133" s="3">
         <v>92.62</v>
@@ -8023,12 +8032,12 @@
         <v>4.2299999999999995</v>
       </c>
     </row>
-    <row r="134" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <v>42675</v>
       </c>
       <c r="B134" s="3">
-        <v>104.60037845530603</v>
+        <v>104.57927825855512</v>
       </c>
       <c r="C134" s="3">
         <v>92.73</v>
@@ -8079,12 +8088,12 @@
         <v>4.18</v>
       </c>
     </row>
-    <row r="135" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
         <v>42705</v>
       </c>
       <c r="B135" s="3">
-        <v>108.27129990664594</v>
+        <v>108.25160840977331</v>
       </c>
       <c r="C135" s="3">
         <v>93.11</v>
@@ -8135,12 +8144,12 @@
         <v>4.3600000000000003</v>
       </c>
     </row>
-    <row r="136" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
         <v>42736</v>
       </c>
       <c r="B136" s="3">
-        <v>105.7834462263922</v>
+        <v>105.78538574317058</v>
       </c>
       <c r="C136" s="3">
         <v>94.07</v>
@@ -8191,12 +8200,12 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="137" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <v>42767</v>
       </c>
       <c r="B137" s="3">
-        <v>102.71358026571293</v>
+        <v>102.72738981891978</v>
       </c>
       <c r="C137" s="3">
         <v>95.01</v>
@@ -8247,12 +8256,12 @@
         <v>4.09</v>
       </c>
     </row>
-    <row r="138" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <v>42795</v>
       </c>
       <c r="B138" s="3">
-        <v>98.549061474373829</v>
+        <v>98.562750363973961</v>
       </c>
       <c r="C138" s="3">
         <v>95.46</v>
@@ -8303,12 +8312,12 @@
         <v>3.85</v>
       </c>
     </row>
-    <row r="139" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <v>42826</v>
       </c>
       <c r="B139" s="3">
-        <v>99.612883556989857</v>
+        <v>99.619382701919633</v>
       </c>
       <c r="C139" s="3">
         <v>95.91</v>
@@ -8359,12 +8368,12 @@
         <v>3.65</v>
       </c>
     </row>
-    <row r="140" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
         <v>42856</v>
       </c>
       <c r="B140" s="3">
-        <v>100.70234531661657</v>
+        <v>100.7017778281346</v>
       </c>
       <c r="C140" s="3">
         <v>96.12</v>
@@ -8415,12 +8424,12 @@
         <v>3.6700000000000004</v>
       </c>
     </row>
-    <row r="141" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
         <v>42887</v>
       </c>
       <c r="B141" s="3">
-        <v>101.42440564131807</v>
+        <v>101.4242953893505</v>
       </c>
       <c r="C141" s="3">
         <v>96.23</v>
@@ -8471,12 +8480,12 @@
         <v>3.62</v>
       </c>
     </row>
-    <row r="142" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
         <v>42917</v>
       </c>
       <c r="B142" s="3">
-        <v>103.54807436171706</v>
+        <v>103.55387632135943</v>
       </c>
       <c r="C142" s="3">
         <v>96.18</v>
@@ -8527,12 +8536,12 @@
         <v>3.5999999999999996</v>
       </c>
     </row>
-    <row r="143" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
         <v>42948</v>
       </c>
       <c r="B143" s="3">
-        <v>104.81917499169303</v>
+        <v>104.82700324727904</v>
       </c>
       <c r="C143" s="3">
         <v>96.32</v>
@@ -8583,12 +8592,12 @@
         <v>3.62</v>
       </c>
     </row>
-    <row r="144" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
         <v>42979</v>
       </c>
       <c r="B144" s="3">
-        <v>104.76000050573698</v>
+        <v>104.76622444487596</v>
       </c>
       <c r="C144" s="3">
         <v>96.36</v>
@@ -8639,12 +8648,12 @@
         <v>3.63</v>
       </c>
     </row>
-    <row r="145" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <v>43009</v>
       </c>
       <c r="B145" s="3">
-        <v>104.46667286169117</v>
+        <v>104.45169428649952</v>
       </c>
       <c r="C145" s="3">
         <v>96.37</v>
@@ -8695,12 +8704,12 @@
         <v>3.63</v>
       </c>
     </row>
-    <row r="146" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
         <v>43040</v>
       </c>
       <c r="B146" s="3">
-        <v>105.51619047951289</v>
+        <v>105.49474445127544</v>
       </c>
       <c r="C146" s="3">
         <v>96.55</v>
@@ -8751,12 +8760,12 @@
         <v>3.54</v>
       </c>
     </row>
-    <row r="147" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
         <v>43070</v>
       </c>
       <c r="B147" s="3">
-        <v>109.68430107938671</v>
+        <v>109.66449850261513</v>
       </c>
       <c r="C147" s="3">
         <v>96.92</v>
@@ -8807,12 +8816,12 @@
         <v>3.46</v>
       </c>
     </row>
-    <row r="148" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
         <v>43101</v>
       </c>
       <c r="B148" s="3">
-        <v>107.28591587001868</v>
+        <v>107.28874897787364</v>
       </c>
       <c r="C148" s="3">
         <v>97.53</v>
@@ -8863,12 +8872,12 @@
         <v>3.42</v>
       </c>
     </row>
-    <row r="149" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <v>43132</v>
       </c>
       <c r="B149" s="3">
-        <v>104.39579042709663</v>
+        <v>104.40973898275469</v>
       </c>
       <c r="C149" s="3">
         <v>98.22</v>
@@ -8919,12 +8928,12 @@
         <v>3.35</v>
       </c>
     </row>
-    <row r="150" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <v>43160</v>
       </c>
       <c r="B150" s="3">
-        <v>100.11894411815285</v>
+        <v>100.13160996251572</v>
       </c>
       <c r="C150" s="3">
         <v>98.45</v>
@@ -8975,12 +8984,12 @@
         <v>3.29</v>
       </c>
     </row>
-    <row r="151" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
         <v>43191</v>
       </c>
       <c r="B151" s="3">
-        <v>102.00593466229644</v>
+        <v>102.0102084278144</v>
       </c>
       <c r="C151" s="3">
         <v>98.91</v>
@@ -9031,12 +9040,12 @@
         <v>3.29</v>
       </c>
     </row>
-    <row r="152" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
         <v>43221</v>
       </c>
       <c r="B152" s="3">
-        <v>103.32771137057439</v>
+        <v>103.32491913561599</v>
       </c>
       <c r="C152" s="3">
         <v>99.16</v>
@@ -9087,12 +9096,12 @@
         <v>3.27</v>
       </c>
     </row>
-    <row r="153" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
         <v>43252</v>
       </c>
       <c r="B153" s="3">
-        <v>104.11174243709638</v>
+        <v>104.10958763778972</v>
       </c>
       <c r="C153" s="3">
         <v>99.31</v>
@@ -9143,12 +9152,12 @@
         <v>3.3099999999999996</v>
       </c>
     </row>
-    <row r="154" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
         <v>43282</v>
       </c>
       <c r="B154" s="3">
-        <v>105.94778926107695</v>
+        <v>105.95196567917071</v>
       </c>
       <c r="C154" s="3">
         <v>99.18</v>
@@ -9199,12 +9208,12 @@
         <v>3.32</v>
       </c>
     </row>
-    <row r="155" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
         <v>43313</v>
       </c>
       <c r="B155" s="3">
-        <v>107.56051576792646</v>
+        <v>107.56702300925436</v>
       </c>
       <c r="C155" s="3">
         <v>99.3</v>
@@ -9255,12 +9264,12 @@
         <v>3.3300000000000005</v>
       </c>
     </row>
-    <row r="156" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
         <v>43344</v>
       </c>
       <c r="B156" s="3">
-        <v>107.75419016035482</v>
+        <v>107.75974917512924</v>
       </c>
       <c r="C156" s="3">
         <v>99.47</v>
@@ -9311,12 +9320,12 @@
         <v>3.37</v>
       </c>
     </row>
-    <row r="157" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
         <v>43374</v>
       </c>
       <c r="B157" s="3">
-        <v>107.64416479452245</v>
+        <v>107.63063961128472</v>
       </c>
       <c r="C157" s="3">
         <v>99.59</v>
@@ -9367,12 +9376,12 @@
         <v>3.37</v>
       </c>
     </row>
-    <row r="158" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
         <v>43405</v>
       </c>
       <c r="B158" s="3">
-        <v>108.83522039079726</v>
+        <v>108.81622829411793</v>
       </c>
       <c r="C158" s="3">
         <v>99.7</v>
@@ -9423,12 +9432,12 @@
         <v>3.6700000000000004</v>
       </c>
     </row>
-    <row r="159" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <v>43435</v>
       </c>
       <c r="B159" s="3">
-        <v>112.85418135489952</v>
+        <v>112.83811129506883</v>
       </c>
       <c r="C159" s="3">
         <v>100</v>
@@ -9479,12 +9488,12 @@
         <v>3.5000000000000004</v>
       </c>
     </row>
-    <row r="160" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
         <v>43466</v>
       </c>
       <c r="B160" s="3">
-        <v>110.40339385930724</v>
+        <v>110.40861261205286</v>
       </c>
       <c r="C160" s="3">
         <v>100.6</v>
@@ -9535,12 +9544,12 @@
         <v>3.4099999999999997</v>
       </c>
     </row>
-    <row r="161" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
         <v>43497</v>
       </c>
       <c r="B161" s="3">
-        <v>107.44976104148655</v>
+        <v>107.46398930817823</v>
       </c>
       <c r="C161" s="3">
         <v>101.18</v>
@@ -9591,12 +9600,12 @@
         <v>3.35</v>
       </c>
     </row>
-    <row r="162" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
         <v>43525</v>
       </c>
       <c r="B162" s="3">
-        <v>103.59974461100683</v>
+        <v>103.61193163805682</v>
       </c>
       <c r="C162" s="3">
         <v>101.62</v>
@@ -9647,12 +9656,12 @@
         <v>3.32</v>
       </c>
     </row>
-    <row r="163" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
         <v>43556</v>
       </c>
       <c r="B163" s="3">
-        <v>105.13310618306194</v>
+        <v>105.13712747611123</v>
       </c>
       <c r="C163" s="3">
         <v>102.12</v>
@@ -9703,12 +9712,12 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="164" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
         <v>43586</v>
       </c>
       <c r="B164" s="3">
-        <v>106.73999788742287</v>
+        <v>106.73891767167144</v>
       </c>
       <c r="C164" s="3">
         <v>102.44</v>
@@ -9759,12 +9768,12 @@
         <v>3.26</v>
       </c>
     </row>
-    <row r="165" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
         <v>43617</v>
       </c>
       <c r="B165" s="3">
-        <v>107.23394402274005</v>
+        <v>107.23347000529448</v>
       </c>
       <c r="C165" s="3">
         <v>102.71</v>
@@ -9815,12 +9824,12 @@
         <v>3.26</v>
       </c>
     </row>
-    <row r="166" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
         <v>43647</v>
       </c>
       <c r="B166" s="3">
-        <v>109.79454924702122</v>
+        <v>109.80008306721494</v>
       </c>
       <c r="C166" s="3">
         <v>102.94</v>
@@ -9871,12 +9880,12 @@
         <v>3.3099999999999996</v>
       </c>
     </row>
-    <row r="167" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
         <v>43678</v>
       </c>
       <c r="B167" s="3">
-        <v>110.87464019540238</v>
+        <v>110.88122547872814</v>
       </c>
       <c r="C167" s="3">
         <v>103.03</v>
@@ -9927,12 +9936,12 @@
         <v>3.36</v>
       </c>
     </row>
-    <row r="168" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
         <v>43709</v>
       </c>
       <c r="B168" s="3">
-        <v>110.92794502446793</v>
+        <v>110.93360362876898</v>
       </c>
       <c r="C168" s="3">
         <v>103.26</v>
@@ -9983,12 +9992,12 @@
         <v>3.35</v>
       </c>
     </row>
-    <row r="169" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
         <v>43739</v>
       </c>
       <c r="B169" s="3">
-        <v>110.43410054659171</v>
+        <v>110.41495207482649</v>
       </c>
       <c r="C169" s="3">
         <v>103.43</v>
@@ -10039,12 +10048,12 @@
         <v>3.37</v>
       </c>
     </row>
-    <row r="170" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
         <v>43770</v>
       </c>
       <c r="B170" s="3">
-        <v>111.59504753272016</v>
+        <v>111.57303038640543</v>
       </c>
       <c r="C170" s="3">
         <v>103.54</v>
@@ -10095,12 +10104,12 @@
         <v>3.4000000000000004</v>
       </c>
     </row>
-    <row r="171" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
         <v>43800</v>
       </c>
       <c r="B171" s="3">
-        <v>116.11211230882594</v>
+        <v>116.09474069492073</v>
       </c>
       <c r="C171" s="3">
         <v>103.8</v>
@@ -10151,12 +10160,12 @@
         <v>3.36</v>
       </c>
     </row>
-    <row r="172" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
         <v>43831</v>
       </c>
       <c r="B172" s="3">
-        <v>113.71063409558167</v>
+        <v>113.71949366342288</v>
       </c>
       <c r="C172" s="3">
         <v>104.24</v>
@@ -10207,12 +10216,12 @@
         <v>3.4099999999999997</v>
       </c>
     </row>
-    <row r="173" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
         <v>43862</v>
       </c>
       <c r="B173" s="3">
-        <v>111.18631684356824</v>
+        <v>111.20064470253767</v>
       </c>
       <c r="C173" s="3">
         <v>104.94</v>
@@ -10263,12 +10272,12 @@
         <v>3.4000000000000004</v>
       </c>
     </row>
-    <row r="174" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
         <v>43891</v>
       </c>
       <c r="B174" s="3">
-        <v>103.88373961882895</v>
+        <v>103.89017055460926</v>
       </c>
       <c r="C174" s="3">
         <v>105.53</v>
@@ -10319,12 +10328,12 @@
         <v>3.52</v>
       </c>
     </row>
-    <row r="175" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
         <v>43922</v>
       </c>
       <c r="B175" s="3">
-        <v>97.156894095227528</v>
+        <v>97.157541611784211</v>
       </c>
       <c r="C175" s="3">
         <v>105.7</v>
@@ -10353,8 +10362,9 @@
       <c r="K175" s="4">
         <v>61.630513636363638</v>
       </c>
-      <c r="L175" s="7">
-        <v>217</v>
+      <c r="L175" s="9">
+        <f>217*0+AVERAGE(L174,L176)</f>
+        <v>10611.5</v>
       </c>
       <c r="M175" s="7">
         <v>1374.0469671399999</v>
@@ -10375,12 +10385,12 @@
         <v>3.38</v>
       </c>
     </row>
-    <row r="176" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
         <v>43952</v>
       </c>
       <c r="B176" s="3">
-        <v>91.113606467734215</v>
+        <v>91.108770509572864</v>
       </c>
       <c r="C176" s="3">
         <v>105.36</v>
@@ -10431,12 +10441,12 @@
         <v>2.94</v>
       </c>
     </row>
-    <row r="177" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
         <v>43983</v>
       </c>
       <c r="B177" s="3">
-        <v>89.294190155208128</v>
+        <v>89.290006510249555</v>
       </c>
       <c r="C177" s="3">
         <v>104.97</v>
@@ -10487,12 +10497,12 @@
         <v>2.88</v>
       </c>
     </row>
-    <row r="178" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
         <v>44013</v>
       </c>
       <c r="B178" s="3">
-        <v>94.958159346499698</v>
+        <v>94.954710356618804</v>
       </c>
       <c r="C178" s="3">
         <v>104.97</v>
@@ -10543,12 +10553,12 @@
         <v>2.85</v>
       </c>
     </row>
-    <row r="179" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
         <v>44044</v>
       </c>
       <c r="B179" s="3">
-        <v>98.498857598773725</v>
+        <v>98.49499723883487</v>
       </c>
       <c r="C179" s="3">
         <v>104.96</v>
@@ -10599,12 +10609,12 @@
         <v>2.7199999999999998</v>
       </c>
     </row>
-    <row r="180" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
         <v>44075</v>
       </c>
       <c r="B180" s="3">
-        <v>100.77098273352654</v>
+        <v>100.76713878925921</v>
       </c>
       <c r="C180" s="3">
         <v>105.29</v>
@@ -10655,12 +10665,12 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="181" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
         <v>44105</v>
       </c>
       <c r="B181" s="3">
-        <v>102.49318816884214</v>
+        <v>102.49014403047391</v>
       </c>
       <c r="C181" s="3">
         <v>105.23</v>
@@ -10711,12 +10721,12 @@
         <v>2.8000000000000003</v>
       </c>
     </row>
-    <row r="182" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
         <v>44136</v>
       </c>
       <c r="B182" s="3">
-        <v>106.0666234975201</v>
+        <v>106.0657315135429</v>
       </c>
       <c r="C182" s="3">
         <v>105.08</v>
@@ -10767,12 +10777,12 @@
         <v>2.8000000000000003</v>
       </c>
     </row>
-    <row r="183" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
         <v>44166</v>
       </c>
       <c r="B183" s="3">
-        <v>111.9787330930376</v>
+        <v>111.98032974648292</v>
       </c>
       <c r="C183" s="3">
         <v>105.48</v>
@@ -10823,12 +10833,12 @@
         <v>2.73</v>
       </c>
     </row>
-    <row r="184" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
         <v>44197</v>
       </c>
       <c r="B184" s="3">
-        <v>110.10841701083507</v>
+        <v>110.11002287981817</v>
       </c>
       <c r="C184" s="3">
         <v>105.91</v>
@@ -10879,12 +10889,12 @@
         <v>2.8000000000000003</v>
       </c>
     </row>
-    <row r="185" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
         <v>44228</v>
       </c>
       <c r="B185" s="3">
-        <v>107.84394767031574</v>
+        <v>107.84218611160622</v>
       </c>
       <c r="C185" s="3">
         <v>106.58</v>
@@ -10935,12 +10945,12 @@
         <v>2.86</v>
       </c>
     </row>
-    <row r="186" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
         <v>44256</v>
       </c>
       <c r="B186" s="3">
-        <v>105.23192178350756</v>
+        <v>105.22401965303213</v>
       </c>
       <c r="C186" s="3">
         <v>107.12</v>
@@ -10991,12 +11001,12 @@
         <v>2.87</v>
       </c>
     </row>
-    <row r="187" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
         <v>44287</v>
       </c>
       <c r="B187" s="3">
-        <v>106.83640843053043</v>
+        <v>106.8277412994961</v>
       </c>
       <c r="C187" s="3">
         <v>107.76</v>
@@ -11047,12 +11057,12 @@
         <v>2.92</v>
       </c>
     </row>
-    <row r="188" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
         <v>44317</v>
       </c>
       <c r="B188" s="3">
-        <v>106.01470260855713</v>
+        <v>106.00978589873107</v>
       </c>
       <c r="C188" s="3">
         <v>108.84</v>
@@ -11103,12 +11113,12 @@
         <v>2.8400000000000003</v>
       </c>
     </row>
-    <row r="189" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
         <v>44348</v>
       </c>
       <c r="B189" s="3">
-        <v>105.35990105208872</v>
+        <v>105.3634297069441</v>
       </c>
       <c r="C189" s="3">
         <v>108.78</v>
@@ -11159,12 +11169,12 @@
         <v>2.97</v>
       </c>
     </row>
-    <row r="190" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
         <v>44378</v>
       </c>
       <c r="B190" s="3">
-        <v>108.28597549934246</v>
+        <v>108.29219348856718</v>
       </c>
       <c r="C190" s="3">
         <v>109.14</v>
@@ -11215,12 +11225,12 @@
         <v>3.18</v>
       </c>
     </row>
-    <row r="191" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
         <v>44409</v>
       </c>
       <c r="B191" s="3">
-        <v>111.70274557510925</v>
+        <v>111.70911449134007</v>
       </c>
       <c r="C191" s="3">
         <v>109.62</v>
@@ -11271,12 +11281,12 @@
         <v>3.2800000000000002</v>
       </c>
     </row>
-    <row r="192" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
         <v>44440</v>
       </c>
       <c r="B192" s="3">
-        <v>113.61628196629431</v>
+        <v>113.61806605617824</v>
       </c>
       <c r="C192" s="3">
         <v>110.04</v>
@@ -11327,12 +11337,12 @@
         <v>3.5000000000000004</v>
       </c>
     </row>
-    <row r="193" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
         <v>44470</v>
       </c>
       <c r="B193" s="3">
-        <v>114.5290879065866</v>
+        <v>114.52414889576448</v>
       </c>
       <c r="C193" s="3">
         <v>110.06</v>
@@ -11383,12 +11393,12 @@
         <v>3.63</v>
       </c>
     </row>
-    <row r="194" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
         <v>44501</v>
       </c>
       <c r="B194" s="3">
-        <v>118.09516461220431</v>
+        <v>118.09329646686433</v>
       </c>
       <c r="C194" s="3">
         <v>110.6</v>
@@ -11439,12 +11449,12 @@
         <v>3.65</v>
       </c>
     </row>
-    <row r="195" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
         <v>44531</v>
       </c>
       <c r="B195" s="3">
-        <v>123.540487683425</v>
+        <v>123.5430770691612</v>
       </c>
       <c r="C195" s="3">
         <v>111.41</v>
@@ -11495,12 +11505,12 @@
         <v>3.91</v>
       </c>
     </row>
-    <row r="196" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
         <v>44562</v>
       </c>
       <c r="B196" s="3">
-        <v>120.85512108992646</v>
+        <v>120.86166507442368</v>
       </c>
       <c r="C196" s="3">
         <v>113.26</v>
@@ -11551,12 +11561,12 @@
         <v>4.03</v>
       </c>
     </row>
-    <row r="197" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A197" s="2">
         <v>44593</v>
       </c>
       <c r="B197" s="3">
-        <v>117.05012543987355</v>
+        <v>117.06659807267177</v>
       </c>
       <c r="C197" s="3">
         <v>115.11</v>
@@ -11607,12 +11617,12 @@
         <v>4.1900000000000004</v>
       </c>
     </row>
-    <row r="198" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A198" s="2">
         <v>44621</v>
       </c>
       <c r="B198" s="3">
-        <v>112.9847514183348</v>
+        <v>113.01040407234227</v>
       </c>
       <c r="C198" s="3">
         <v>116.26</v>
@@ -11663,12 +11673,12 @@
         <v>4.55</v>
       </c>
     </row>
-    <row r="199" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A199" s="2">
         <v>44652</v>
       </c>
       <c r="B199" s="3">
-        <v>115.44440172675552</v>
+        <v>115.4769157269767</v>
       </c>
       <c r="C199" s="3">
         <v>117.71</v>
@@ -11719,12 +11729,12 @@
         <v>4.63</v>
       </c>
     </row>
-    <row r="200" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A200" s="2">
         <v>44682</v>
       </c>
       <c r="B200" s="3">
-        <v>117.99954064935982</v>
+        <v>118.01628509505447</v>
       </c>
       <c r="C200" s="3">
         <v>118.7</v>
@@ -11775,12 +11785,12 @@
         <v>5.2299999999999995</v>
       </c>
     </row>
-    <row r="201" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A201" s="2">
         <v>44713</v>
       </c>
       <c r="B201" s="3">
-        <v>117.56745602960467</v>
+        <v>117.56214192849329</v>
       </c>
       <c r="C201" s="3">
         <v>119.31</v>
@@ -11831,12 +11841,12 @@
         <v>5.48</v>
       </c>
     </row>
-    <row r="202" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A202" s="2">
         <v>44743</v>
       </c>
       <c r="B202" s="3">
-        <v>119.20876595660646</v>
+        <v>119.19117191587607</v>
       </c>
       <c r="C202" s="3">
         <v>120.27</v>
@@ -11887,12 +11897,12 @@
         <v>5.86</v>
       </c>
     </row>
-    <row r="203" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A203" s="2">
         <v>44774</v>
       </c>
       <c r="B203" s="3">
-        <v>120.15888911137382</v>
+        <v>120.13134984102767</v>
       </c>
       <c r="C203" s="3">
         <v>121.5</v>
@@ -11943,12 +11953,12 @@
         <v>6.1400000000000006</v>
       </c>
     </row>
-    <row r="204" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A204" s="2">
         <v>44805</v>
       </c>
       <c r="B204" s="3">
-        <v>120.867891515783</v>
+        <v>120.84108081503177</v>
       </c>
       <c r="C204" s="3">
         <v>122.63</v>
@@ -11999,12 +12009,12 @@
         <v>7.0499999999999989</v>
       </c>
     </row>
-    <row r="205" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A205" s="2">
         <v>44835</v>
       </c>
       <c r="B205" s="3">
-        <v>120.79573815999247</v>
+        <v>120.82509578064584</v>
       </c>
       <c r="C205" s="3">
         <v>123.51</v>
@@ -12055,12 +12065,12 @@
         <v>7.3800000000000008</v>
       </c>
     </row>
-    <row r="206" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A206" s="2">
         <v>44866</v>
       </c>
       <c r="B206" s="3">
-        <v>121.06594243787636</v>
+        <v>121.08809521743269</v>
       </c>
       <c r="C206" s="3">
         <v>124.46</v>
@@ -12111,12 +12121,12 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="207" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A207" s="2">
         <v>44896</v>
       </c>
       <c r="B207" s="3">
-        <v>124.99429416577154</v>
+        <v>125.0007663136267</v>
       </c>
       <c r="C207" s="3">
         <v>126.03</v>
@@ -12167,12 +12177,12 @@
         <v>7.7399999999999993</v>
       </c>
     </row>
-    <row r="208" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A208" s="2">
         <v>44927</v>
       </c>
       <c r="B208" s="3">
-        <v>122.30827265848988</v>
+        <v>122.23813080719985</v>
       </c>
       <c r="C208" s="3">
         <v>128.27000000000001</v>
@@ -12223,12 +12233,12 @@
         <v>7.86</v>
       </c>
     </row>
-    <row r="209" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A209" s="2">
         <v>44958</v>
       </c>
       <c r="B209" s="3">
-        <v>119.32406665176212</v>
+        <v>119.23778048802895</v>
       </c>
       <c r="C209" s="3">
         <v>130.4</v>
@@ -12279,12 +12289,12 @@
         <v>7.31</v>
       </c>
     </row>
-    <row r="210" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
         <v>44986</v>
       </c>
       <c r="B210" s="3">
-        <v>115.58752818067556</v>
+        <v>115.4854970571209</v>
       </c>
       <c r="C210" s="3">
         <v>131.77000000000001</v>
@@ -12335,12 +12345,12 @@
         <v>7.32</v>
       </c>
     </row>
-    <row r="211" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A211" s="2">
         <v>45017</v>
       </c>
       <c r="B211" s="3">
-        <v>116.30781413695563</v>
+        <v>116.19847391141134</v>
       </c>
       <c r="C211" s="3">
         <v>132.80000000000001</v>
@@ -12391,12 +12401,12 @@
         <v>7.03</v>
       </c>
     </row>
-    <row r="212" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A212" s="2">
         <v>45047</v>
       </c>
       <c r="B212" s="3">
-        <v>118.01678127188177</v>
+        <v>117.9024804921487</v>
       </c>
       <c r="C212" s="3">
         <v>133.38</v>
@@ -12447,12 +12457,12 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="213" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
         <v>45078</v>
       </c>
       <c r="B213" s="3">
-        <v>117.81717711413556</v>
+        <v>117.69954760799358</v>
       </c>
       <c r="C213" s="3">
         <v>133.78</v>
@@ -12503,12 +12513,12 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="214" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
         <v>45108</v>
       </c>
       <c r="B214" s="3">
-        <v>119.94695914317636</v>
+        <v>119.83207289672741</v>
       </c>
       <c r="C214" s="3">
         <v>134.44999999999999</v>
@@ -12559,12 +12569,12 @@
         <v>6.15</v>
       </c>
     </row>
-    <row r="215" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A215" s="2">
         <v>45139</v>
       </c>
       <c r="B215" s="3">
-        <v>120.98219453968998</v>
+        <v>120.87949162515838</v>
       </c>
       <c r="C215" s="3">
         <v>135.38999999999999</v>
@@ -12615,12 +12625,12 @@
         <v>6.04</v>
       </c>
     </row>
-    <row r="216" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A216" s="2">
         <v>45170</v>
       </c>
       <c r="B216" s="3">
-        <v>120.38564262641098</v>
+        <v>120.43006818377883</v>
       </c>
       <c r="C216" s="3">
         <v>136.11000000000001</v>
@@ -12671,12 +12681,12 @@
         <v>6.05</v>
       </c>
     </row>
-    <row r="217" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A217" s="2">
         <v>45200</v>
       </c>
       <c r="B217" s="3">
-        <v>119.78257805975416</v>
+        <v>119.8862339956885</v>
       </c>
       <c r="C217" s="3">
         <v>136.44999999999999</v>
@@ -12727,12 +12737,12 @@
         <v>5.89</v>
       </c>
     </row>
-    <row r="218" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A218" s="2">
         <v>45231</v>
       </c>
       <c r="B218" s="3">
-        <v>120.99512631705505</v>
+        <v>121.23488580356498</v>
       </c>
       <c r="C218" s="3">
         <v>137.09</v>
@@ -12783,12 +12793,12 @@
         <v>5.72</v>
       </c>
     </row>
-    <row r="219" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A219" s="2">
         <v>45261</v>
       </c>
       <c r="B219" s="3">
-        <v>125.61809525425333</v>
+        <v>125.79333032658218</v>
       </c>
       <c r="C219" s="3">
         <v>137.72</v>
@@ -12839,12 +12849,12 @@
         <v>5.6099999999999994</v>
       </c>
     </row>
-    <row r="220" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A220" s="2">
         <v>45292</v>
       </c>
       <c r="B220" s="3">
-        <v>123.93974357916365</v>
+        <v>124.08552434775955</v>
       </c>
       <c r="C220" s="3">
         <v>138.97999999999999</v>
@@ -12895,12 +12905,12 @@
         <v>5.13</v>
       </c>
     </row>
-    <row r="221" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A221" s="2">
         <v>45323</v>
       </c>
       <c r="B221" s="3">
-        <v>120.83956304751079</v>
+        <v>120.93398063818252</v>
       </c>
       <c r="C221" s="3">
         <v>140.49</v>
@@ -12951,12 +12961,12 @@
         <v>4.83</v>
       </c>
     </row>
-    <row r="222" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A222" s="2">
         <v>45352</v>
       </c>
       <c r="B222" s="3">
-        <v>116.60145854684102</v>
+        <v>116.3311913144132</v>
       </c>
       <c r="C222" s="3">
         <v>141.47999999999999</v>
@@ -13007,12 +13017,12 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="223" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
         <v>45383</v>
       </c>
       <c r="B223" s="3">
-        <v>118.91942724853054</v>
+        <v>118.6797536804218</v>
       </c>
       <c r="C223" s="3">
         <v>142.32</v>
@@ -13063,12 +13073,12 @@
         <v>4.67</v>
       </c>
     </row>
-    <row r="224" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A224" s="2">
         <v>45413</v>
       </c>
       <c r="B224" s="3">
-        <v>120.70374317352848</v>
+        <v>120.43052369299299</v>
       </c>
       <c r="C224" s="3">
         <v>142.91999999999999</v>
@@ -13119,12 +13129,12 @@
         <v>4.58</v>
       </c>
     </row>
-    <row r="225" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A225" s="2">
         <v>45444</v>
       </c>
       <c r="B225" s="3">
-        <v>120.49667341794789</v>
+        <v>120.40611789679572</v>
       </c>
       <c r="C225" s="3">
         <v>143.38</v>
@@ -13175,12 +13185,12 @@
         <v>4.37</v>
       </c>
     </row>
-    <row r="226" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A226" s="2">
         <v>45474</v>
       </c>
       <c r="B226" s="3">
-        <v>121.98588493730944</v>
+        <v>121.70257510847411</v>
       </c>
       <c r="C226" s="3">
         <v>143.66999999999999</v>
@@ -13231,12 +13241,12 @@
         <v>4.29</v>
       </c>
     </row>
-    <row r="227" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A227" s="2">
         <v>45505</v>
       </c>
       <c r="B227" s="3">
-        <v>122.91148941944341</v>
+        <v>122.39307341199127</v>
       </c>
       <c r="C227" s="3">
         <v>143.66999999999999</v>
@@ -13287,10 +13297,13 @@
         <v>4.16</v>
       </c>
     </row>
-    <row r="228" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A228" s="2">
         <v>45536</v>
       </c>
+      <c r="B228" s="3">
+        <v>122.94307645308739</v>
+      </c>
       <c r="C228" s="3">
         <v>144.02000000000001</v>
       </c>
@@ -13340,7 +13353,7 @@
         <v>4.1900000000000004</v>
       </c>
     </row>
-    <row r="229" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A229" s="2">
         <v>45566</v>
       </c>

</xml_diff>